<commit_message>
test d'un jeu de données pour exo
</commit_message>
<xml_diff>
--- a/Exercices/01 - Concevoir une base de données/01 - Concevoir une base de données/99 - Divers/11 - IGPN.xlsx
+++ b/Exercices/01 - Concevoir une base de données/01 - Concevoir une base de données/99 - Divers/11 - IGPN.xlsx
@@ -1,18 +1,152 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF53410F-BA0F-4DFC-9398-E8B4D8B3E8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau101" hidden="1">Tableau10[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau21" hidden="1">Tableau2[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau31" hidden="1">Tableau3[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau41" hidden="1">Tableau4[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau51" hidden="1">Tableau5[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau61" hidden="1">Tableau6[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau71" hidden="1">Tableau7[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau81" hidden="1">Tableau8[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_11IGPN.xlsxTableau91" hidden="1">Tableau9[]</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Tableau2" name="Tableau2" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau2"/>
+          <x15:modelTable id="Tableau10" name="Tableau10" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau10"/>
+          <x15:modelTable id="Tableau3" name="Tableau3" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau3"/>
+          <x15:modelTable id="Tableau7" name="Tableau7" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau7"/>
+          <x15:modelTable id="Tableau4" name="Tableau4" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau4"/>
+          <x15:modelTable id="Tableau8" name="Tableau8" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau8"/>
+          <x15:modelTable id="Tableau5" name="Tableau5" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau5"/>
+          <x15:modelTable id="Tableau6" name="Tableau6" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau6"/>
+          <x15:modelTable id="Tableau9" name="Tableau9" connection="WorksheetConnection_11 - IGPN.xlsx!Tableau9"/>
+        </x15:modelTables>
+        <x15:modelRelationships>
+          <x15:modelRelationship fromTable="Tableau10" fromColumn="#idBlame" toTable="Tableau2" toColumn="idBlame"/>
+          <x15:modelRelationship fromTable="Tableau10" fromColumn="#idPolicier" toTable="Tableau7" toColumn="idPolicier"/>
+          <x15:modelRelationship fromTable="Tableau7" fromColumn="#idGrade" toTable="Tableau3" toColumn="idGrade"/>
+          <x15:modelRelationship fromTable="Tableau7" fromColumn="#idService" toTable="Tableau6" toColumn="idService"/>
+          <x15:modelRelationship fromTable="Tableau8" fromColumn="#idVille" toTable="Tableau4" toColumn="idVille"/>
+          <x15:modelRelationship fromTable="Tableau8" fromColumn="#idCommissariat" toTable="Tableau5" toColumn="idCommissariat"/>
+          <x15:modelRelationship fromTable="Tableau9" fromColumn="#idService" toTable="Tableau6" toColumn="idService"/>
+          <x15:modelRelationship fromTable="Tableau9" fromColumn="#idCommissariat" toTable="Tableau5" toColumn="idCommissariat"/>
+        </x15:modelRelationships>
+      </x15:dataModel>
+    </ext>
+  </extLst>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{8E8826C5-0A0C-4F7B-83AE-3D291A432BD9}" keepAlive="1" name="ThisWorkbookDataModel" description="Modèle de données" type="5" refreshedVersion="8" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" xr16:uid="{0694A848-90AE-43D9-8A5A-567369E089AB}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau10" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau10">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau101"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="3" xr16:uid="{9FAEFC15-5BF7-4A6D-9327-971A43F9FCC7}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau2" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau2">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau21"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="4" xr16:uid="{403F4668-0763-4E3A-AA7D-7F143FCC8990}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau3" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau3">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau31"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="5" xr16:uid="{762A6DF9-4A1B-474F-89F6-7798392CEF75}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau4" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau4">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau41"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="6" xr16:uid="{21E06EC4-5EA5-470E-BC2D-D23F2257356A}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau5" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau5">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau51"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="7" xr16:uid="{96F99B56-2290-47D1-A6F5-1CBAF492FDF9}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau6" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau6">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau61"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="8" xr16:uid="{D2341873-A66D-4D6D-9B62-CBCC34B7F995}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau7" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau7">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau71"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="9" xr16:uid="{ECAA65BA-F4C2-4687-B961-F57C3F3D75D8}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau8" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau8">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau81"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="10" xr16:uid="{E4E020BB-E9B9-40B3-8A65-C3071C3B2BC4}" name="WorksheetConnection_11 - IGPN.xlsx!Tableau9" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Tableau9">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_11IGPN.xlsxTableau91"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -168,18 +302,18 @@
     <t>Barnaby</t>
   </si>
   <si>
-    <t>Clousseau</t>
-  </si>
-  <si>
-    <t>Barnaby travaille au service enquete criminelle du commissariat de lille2 à lille</t>
+    <t>Moulinsard</t>
+  </si>
+  <si>
+    <t>Clouseau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -390,44 +524,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="7" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="7" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20 % - Accent3" xfId="4" builtinId="38"/>
@@ -443,7 +577,7 @@
   </cellStyles>
   <dxfs count="36">
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -460,12 +594,136 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -488,6 +746,72 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -498,30 +822,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -531,6 +844,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -553,20 +873,28 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -576,26 +904,16 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -608,6 +926,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -633,6 +957,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -677,20 +1004,35 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -700,54 +1042,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -757,167 +1051,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -979,103 +1113,216 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A814EC92-F704-5E7E-8C77-C3E78F23EB16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="6105525"/>
+          <a:ext cx="15240000" cy="1666875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Inspecteur Barnaby travaille au service enquete criminelle du commissariat de lille2 à lille et n'a jamais reçu de blame.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>les bleu Dupond</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> et Dupont sont rattachés au service de la voirie du commissariat de moulinsard de Paris et alterne les retards depuis une semaine,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>chef Clouseau s'est redu coupable d'incivilité lors de sa patrouille pour le commissariat de la Croix Rousse de Lyon d'il y a un mois, menant à une plainte pour coups et blessures de la part du suspect qu'il a pris en chasse à cette occasion,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Problèmes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>policiers n'ont que nom, pas de prenom ou de n° matricule =&gt; pas demandé dans l'expression des besoins mais semblait logique</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>policiers n'ont pas de rapport direct avec commissariat ni ville, seulement service =&gt; ma faute, présentes au début mais lors des questions j'ai par erreur dit qu'elles n'étaient pas nécessaire. je me rend compte maintenant que la façon dont je l'ai expliqué (reflèté dans le MCD), causera le besoin de doublons dans la table Service. De plus, pour fonctionner sous cette forme, un service devrait n'êtrepossédé que par un et un seul commissariat et que ce dernier doive être hebergé que par une et une seule ville, sinon on ne peut faire le lien entre policier jusqu'a ville</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A2:B15" totalsRowShown="0" headerRowDxfId="35">
-  <autoFilter ref="A2:B15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau2" displayName="Tableau2" ref="A2:B15" totalsRowShown="0" headerRowDxfId="35">
+  <autoFilter ref="A2:B15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idBlame" dataDxfId="34"/>
-    <tableColumn id="2" name="nomBlame" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="idBlame" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="nomBlame" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="D2:E15" totalsRowShown="0" headerRowDxfId="28">
-  <autoFilter ref="D2:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau3" displayName="Tableau3" ref="D2:E15" totalsRowShown="0" headerRowDxfId="32">
+  <autoFilter ref="D2:E15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idGrade" dataDxfId="32"/>
-    <tableColumn id="2" name="nomGrade" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="idGrade" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="nomGrade" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A18:B31" totalsRowShown="0" headerRowDxfId="27">
-  <autoFilter ref="A18:B31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau4" displayName="Tableau4" ref="A18:B31" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A18:B31" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idVille" dataDxfId="30"/>
-    <tableColumn id="2" name="nomVille" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="idVille" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="nomVille" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="D18:E31" totalsRowShown="0" headerRowDxfId="26">
-  <autoFilter ref="D18:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau5" displayName="Tableau5" ref="D18:E31" totalsRowShown="0" headerRowDxfId="26">
+  <autoFilter ref="D18:E31" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idCommissariat" dataDxfId="25"/>
-    <tableColumn id="2" name="nomCommissariat" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="idCommissariat" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="nomCommissariat" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="G2:H15" totalsRowShown="0">
-  <autoFilter ref="G2:H15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau6" displayName="Tableau6" ref="G2:H15" totalsRowShown="0">
+  <autoFilter ref="G2:H15" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idService" dataDxfId="23"/>
-    <tableColumn id="2" name="nomService" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="idService" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="nomService" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="G18:J31" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
-  <autoFilter ref="G18:J31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tableau7" displayName="Tableau7" ref="G18:J31" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="G18:J31" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="idPolicier" dataDxfId="18"/>
-    <tableColumn id="2" name="nomPolicier" dataDxfId="16"/>
-    <tableColumn id="3" name="#idGrade" dataDxfId="15"/>
-    <tableColumn id="4" name="#idService" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="idPolicier" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="nomPolicier" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="#idGrade" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="#idService" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="L2:M15" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5" headerRowCellStyle="Neutre" dataCellStyle="Neutre">
-  <autoFilter ref="L2:M15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tableau8" displayName="Tableau8" ref="L2:M15" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="L2:M15" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="#idVille" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="#idCommissariat" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="#idVille" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="#idCommissariat" dataDxfId="8" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="L18:M31" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="L18:M31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tableau9" displayName="Tableau9" ref="L18:M31" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="L18:M31" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="#idCommissariat" dataDxfId="10"/>
-    <tableColumn id="2" name="#idService" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="#idCommissariat" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="#idService" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="O2:Q15" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="O2:Q15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tableau10" displayName="Tableau10" ref="O2:Q15" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="O2:Q15" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="#idBlame"/>
-    <tableColumn id="2" name="#idPolicier"/>
-    <tableColumn id="3" name="dateBlame" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="#idBlame"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="#idPolicier"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="dateBlame" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1157,6 +1404,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1192,6 +1456,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1367,11 +1648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,8 +1663,8 @@
     <col min="5" max="5" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" customWidth="1"/>
     <col min="12" max="13" width="17.85546875" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
@@ -1392,27 +1673,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="L1" s="17" t="s">
+      <c r="H1" s="22"/>
+      <c r="L1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="O1" s="2" t="s">
+      <c r="M1" s="16"/>
+      <c r="O1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1434,10 +1715,10 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="1"/>
@@ -1455,267 +1736,351 @@
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="22"/>
-      <c r="Q3" s="23"/>
+      <c r="L3" s="10">
+        <v>2</v>
+      </c>
+      <c r="M3" s="14">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>44875</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="10"/>
-      <c r="Q4" s="23"/>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>44876</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="22"/>
-      <c r="Q5" s="23"/>
+      <c r="L5" s="10">
+        <v>4</v>
+      </c>
+      <c r="M5" s="14">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>44877</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="G6" s="6">
+      <c r="E6" s="2"/>
+      <c r="G6" s="2">
         <v>4</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="10"/>
-      <c r="Q6" s="23"/>
+      <c r="H6" s="2"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="4"/>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>44878</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="G7" s="6">
+      <c r="E7" s="2"/>
+      <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="22"/>
-      <c r="Q7" s="23"/>
+      <c r="H7" s="2"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="14"/>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>44879</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="D8" s="6">
+      <c r="B8" s="2"/>
+      <c r="D8" s="2">
         <v>6</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="G8" s="6">
+      <c r="E8" s="2"/>
+      <c r="G8" s="2">
         <v>6</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="10"/>
-      <c r="Q8" s="23"/>
+      <c r="H8" s="2"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="4"/>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="15">
+        <v>44880</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="D9" s="6">
+      <c r="B9" s="2"/>
+      <c r="D9" s="2">
         <v>7</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="G9" s="6">
+      <c r="E9" s="2"/>
+      <c r="G9" s="2">
         <v>7</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="22"/>
-      <c r="Q9" s="23"/>
+      <c r="H9" s="2"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="14"/>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>44881</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="D10" s="6">
+      <c r="B10" s="2"/>
+      <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="G10" s="6">
+      <c r="E10" s="2"/>
+      <c r="G10" s="2">
         <v>8</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="10"/>
-      <c r="Q10" s="23"/>
+      <c r="H10" s="2"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="4"/>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>44851</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="D11" s="6">
+      <c r="B11" s="2"/>
+      <c r="D11" s="2">
         <v>9</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="G11" s="6">
+      <c r="E11" s="2"/>
+      <c r="G11" s="2">
         <v>9</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="22"/>
-      <c r="Q11" s="23"/>
+      <c r="H11" s="2"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="14"/>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>44851</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="D12" s="6">
+      <c r="B12" s="2"/>
+      <c r="D12" s="2">
         <v>10</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="G12" s="6">
+      <c r="E12" s="2"/>
+      <c r="G12" s="2">
         <v>10</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="10"/>
-      <c r="Q12" s="23"/>
+      <c r="H12" s="2"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="4"/>
+      <c r="Q12" s="15"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="D13" s="6">
+      <c r="B13" s="2"/>
+      <c r="D13" s="2">
         <v>11</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="G13" s="6">
+      <c r="E13" s="2"/>
+      <c r="G13" s="2">
         <v>11</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="22"/>
-      <c r="Q13" s="23"/>
+      <c r="H13" s="2"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="14"/>
+      <c r="Q13" s="15"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="D14" s="6">
+      <c r="B14" s="2"/>
+      <c r="D14" s="2">
         <v>12</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="G14" s="6">
+      <c r="E14" s="2"/>
+      <c r="G14" s="2">
         <v>12</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="10"/>
-      <c r="Q14" s="23"/>
+      <c r="H14" s="2"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="4"/>
+      <c r="Q14" s="15"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="D15" s="6">
+      <c r="B15" s="2"/>
+      <c r="D15" s="2">
         <v>13</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="G15" s="6">
+      <c r="E15" s="2"/>
+      <c r="G15" s="2">
         <v>13</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="21"/>
-      <c r="Q15" s="23"/>
+      <c r="H15" s="2"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="13"/>
+      <c r="Q15" s="15"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="D17" s="7" t="s">
+      <c r="B17" s="20"/>
+      <c r="D17" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="15" t="s">
+      <c r="E17" s="21"/>
+      <c r="G17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="L17" s="4" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="L17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="4"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1731,287 +2096,312 @@
       <c r="E18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="12" t="s">
+      <c r="M18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="10"/>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>3</v>
+      </c>
+      <c r="M19" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="2">
         <v>2</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="3">
         <v>2</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="10"/>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>5</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="2">
         <v>3</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="3">
         <v>3</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="10"/>
+      <c r="I21" s="2">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="2">
         <v>4</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="3">
         <v>4</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="2">
+        <v>3</v>
+      </c>
+      <c r="J22" s="2">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="10"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="G23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="D23" s="6">
-        <v>5</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="G23" s="9">
-        <v>5</v>
-      </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="10"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="2">
         <v>6</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="D24" s="6">
+      <c r="B24" s="2"/>
+      <c r="D24" s="2">
         <v>6</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="G24" s="9">
+      <c r="E24" s="2"/>
+      <c r="G24" s="3">
         <v>6</v>
       </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="10"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="D25" s="6">
+      <c r="B25" s="2"/>
+      <c r="D25" s="2">
         <v>7</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="G25" s="9">
+      <c r="E25" s="2"/>
+      <c r="G25" s="3">
         <v>7</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="10"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="D26" s="6">
+      <c r="B26" s="2"/>
+      <c r="D26" s="2">
         <v>8</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="G26" s="9">
+      <c r="E26" s="2"/>
+      <c r="G26" s="3">
         <v>8</v>
       </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="10"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="D27" s="6">
+      <c r="B27" s="2"/>
+      <c r="D27" s="2">
         <v>9</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="G27" s="9">
+      <c r="E27" s="2"/>
+      <c r="G27" s="3">
         <v>9</v>
       </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="10"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="4"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="D28" s="6">
+      <c r="B28" s="2"/>
+      <c r="D28" s="2">
         <v>10</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="G28" s="9">
+      <c r="E28" s="2"/>
+      <c r="G28" s="3">
         <v>10</v>
       </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="10"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="D29" s="6">
+      <c r="B29" s="2"/>
+      <c r="D29" s="2">
         <v>11</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="G29" s="9">
+      <c r="E29" s="2"/>
+      <c r="G29" s="3">
         <v>11</v>
       </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="10"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="D30" s="6">
+      <c r="B30" s="2"/>
+      <c r="D30" s="2">
         <v>12</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="G30" s="9">
+      <c r="E30" s="2"/>
+      <c r="G30" s="3">
         <v>12</v>
       </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="10"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="4"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="2">
         <v>13</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="D31" s="6">
+      <c r="B31" s="2"/>
+      <c r="D31" s="2">
         <v>13</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="G31" s="9">
+      <c r="E31" s="2"/>
+      <c r="G31" s="3">
         <v>13</v>
       </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2027,8 +2417,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="9">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -2037,12 +2427,13 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2054,7 +2445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>